<commit_message>
Update CDISC Pilot and Diabetes study for USDM 3.6
</commit_message>
<xml_diff>
--- a/Documents/Examples/NCT03421379_EliLilly_Diabetes/EliLilly_NCT03421379_Diabetes.xlsx
+++ b/Documents/Examples/NCT03421379_EliLilly_Diabetes/EliLilly_NCT03421379_Diabetes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/NCT03421379/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm_data/source_data/protocols/NCT03421379_EliLilly_Diabetes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000017C4-49F9-6F41-BB44-C51416FCE056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{672EC8C9-2A8F-CE46-8E21-17F791AC46AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29000" yWindow="500" windowWidth="61640" windowHeight="27180" firstSheet="5" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29000" yWindow="500" windowWidth="61640" windowHeight="27180" firstSheet="4" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="1" r:id="rId1"/>
@@ -2874,45 +2874,6 @@
   </si>
   <si>
     <t>NCI_25</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;This study involves a comparison of 3 mg of LY900018 administered once nasally to 1 mg glucagon administered IM (comparator). Table IGBJ.2 shows the study treatment information.&lt;/p&gt;
-&lt;p&gt;&lt;b&gt;Table IGBJ.2. Study Treatments&lt;/b&gt;&lt;/p&gt;
-&lt;table class="table"&gt;
-  &lt;tr&gt;
-    &lt;th&gt;&lt;p&gt;Treatment Name&lt;/p&gt;&lt;/th&gt;
-    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="StudyIntervention", name="LY" attribute="label"/&gt;&lt;/p&gt;&lt;/td&gt;
-    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="StudyIntervention", name="IMG" attribute="label"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th&gt;&lt;p&gt;Dosage Formulation&lt;/p&gt;&lt;/th&gt;
-    &lt;td&gt;&lt;p&gt;Dry powder&lt;/p&gt;&lt;/td&gt;
-    &lt;td&gt;&lt;p&gt;Dry powder&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th&gt;&lt;p&gt;Dosage Levels  &lt;/p&gt;&lt;/th&gt;
-    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="AgentAdministration", name="LY_ADMIN" attribute="dose/Quantity/@value"/&gt; &lt;usdm:macro id="xref" klass="AgentAdministration", name="LY_ADMIN" attribute="dose/Quantity/@unit/AliasCode/@standardCode/Code/@decode"/&gt; glucagon&lt;/p&gt;&lt;/td&gt;
-    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="AgentAdministration", name="IMG_ADMIN" attribute="dose/Quantity/@value"/&gt; &lt;usdm:macro id="xref" klass="AgentAdministration", name="IMG_ADMIN" attribute="dose/Quantity/@unit/AliasCode/@standardCode/Code/@decode"/&gt; glucagon&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th&gt;&lt;p&gt;Route of Administration&lt;/p&gt;&lt;/th&gt;
-    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="AgentAdministration", name="LY_ADMIN" attribute="@route/AliasCode/@standardCode/Code/@decode"/&gt;&lt;/p&gt;&lt;/td&gt;
-    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="AgentAdministration", name="IMG_ADMIN" attribute="@route/AliasCode/@standardCode/Code/@decode"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;th&gt;&lt;/p&gt;Dosing Instructions&lt;/p&gt;&lt;/th&gt;
-    &lt;td&gt;&lt;/p&gt;&lt;usdm:macro id="xref" klass="AgentAdministration", name="LY_ADMIN" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
-    &lt;td&gt;&lt;/p&gt;&lt;usdm:macro id="xref" klass="AgentAdministration", name="IMG_ADMIN" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-&lt;/table&gt;
-&lt;p&gt;The procedure for insulin-induced hypoglycemia will require an IV infusion of diluted human regular insulin (0.3 U/mL by diluting 15 U human regular insulin [100 U/mL] into 50 mL saline). Details regarding hypoglycemia induction and glucagon administration procedures are included in Sections 9.2.1 and 9.2.2, respectively.&lt;/p&gt;
-&lt;p&gt;The investigator or designee is responsible for:&lt;/p&gt;
-&lt;ul&gt;
-  &lt;li&gt;&lt;p&gt;explaining the correct use of the investigational products to the site personnel&lt;/p&gt;&lt;/li&gt;
-  &lt;li&gt;&lt;p&gt;verifying that instructions are followed properly&lt;/p&gt;&lt;/li&gt;
-  &lt;li&gt;&lt;p&gt;maintaining accurate records of investigational product dispensing and collection&lt;/p&gt;&lt;/li&gt;
-  &lt;li&gt;&lt;p&gt;and returning all unused medication to Lilly or its designee at the end of the study&lt;/p&gt;&lt;/li&gt;
-&lt;/ul&gt;</t>
   </si>
   <si>
     <t>NCI_26</t>
@@ -5585,6 +5546,45 @@
     &lt;/div&gt;
   &lt;/div&gt;
 &lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;This study involves a comparison of 3 mg of LY900018 administered once nasally to 1 mg glucagon administered IM (comparator). Table IGBJ.2 shows the study treatment information.&lt;/p&gt;
+&lt;p&gt;&lt;b&gt;Table IGBJ.2. Study Treatments&lt;/b&gt;&lt;/p&gt;
+&lt;table class="table"&gt;
+  &lt;tr&gt;
+    &lt;th&gt;&lt;p&gt;Treatment Name&lt;/p&gt;&lt;/th&gt;
+    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="StudyIntervention", name="LY" attribute="label"/&gt;&lt;/p&gt;&lt;/td&gt;
+    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="StudyIntervention", name="IMG" attribute="label"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th&gt;&lt;p&gt;Dosage Formulation&lt;/p&gt;&lt;/th&gt;
+    &lt;td&gt;&lt;p&gt;Dry powder&lt;/p&gt;&lt;/td&gt;
+    &lt;td&gt;&lt;p&gt;Dry powder&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th&gt;&lt;p&gt;Dosage Levels  &lt;/p&gt;&lt;/th&gt;
+    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="Administration", name="LY_ADMIN" attribute="dose/Quantity/@value"/&gt; &lt;usdm:macro id="xref" klass="Administration", name="LY_ADMIN" attribute="dose/Quantity/@unit/AliasCode/@standardCode/Code/@decode"/&gt; glucagon&lt;/p&gt;&lt;/td&gt;
+    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="Administration", name="IMG_ADMIN" attribute="dose/Quantity/@value"/&gt; &lt;usdm:macro id="xref" klass="Administration", name="IMG_ADMIN" attribute="dose/Quantity/@unit/AliasCode/@standardCode/Code/@decode"/&gt; glucagon&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th&gt;&lt;p&gt;Route of Administration&lt;/p&gt;&lt;/th&gt;
+    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="Administration", name="LY_ADMIN" attribute="@route/AliasCode/@standardCode/Code/@decode"/&gt;&lt;/p&gt;&lt;/td&gt;
+    &lt;td&gt;&lt;p&gt;&lt;usdm:macro id="xref" klass="Administration", name="IMG_ADMIN" attribute="@route/AliasCode/@standardCode/Code/@decode"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+  &lt;tr&gt;
+    &lt;th&gt;&lt;/p&gt;Dosing Instructions&lt;/p&gt;&lt;/th&gt;
+    &lt;td&gt;&lt;/p&gt;&lt;usdm:macro id="xref" klass="Administration", name="LY_ADMIN" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
+    &lt;td&gt;&lt;/p&gt;&lt;usdm:macro id="xref" klass="Administration", name="IMG_ADMIN" attribute="description"/&gt;&lt;/p&gt;&lt;/td&gt;
+  &lt;/tr&gt;
+&lt;/table&gt;
+&lt;p&gt;The procedure for insulin-induced hypoglycemia will require an IV infusion of diluted human regular insulin (0.3 U/mL by diluting 15 U human regular insulin [100 U/mL] into 50 mL saline). Details regarding hypoglycemia induction and glucagon administration procedures are included in Sections 9.2.1 and 9.2.2, respectively.&lt;/p&gt;
+&lt;p&gt;The investigator or designee is responsible for:&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li&gt;&lt;p&gt;explaining the correct use of the investigational products to the site personnel&lt;/p&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;p&gt;verifying that instructions are followed properly&lt;/p&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;p&gt;maintaining accurate records of investigational product dispensing and collection&lt;/p&gt;&lt;/li&gt;
+  &lt;li&gt;&lt;p&gt;and returning all unused medication to Lilly or its designee at the end of the study&lt;/p&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -10350,8 +10350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10370,12 +10370,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>765</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="409.5" x14ac:dyDescent="0.2">
@@ -10558,672 +10558,672 @@
         <v>809</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>810</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>811</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
+        <v>812</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>813</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
+        <v>814</v>
+      </c>
+      <c r="B29" s="25" t="s">
         <v>815</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
+        <v>816</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>817</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
+        <v>818</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>819</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
+        <v>820</v>
+      </c>
+      <c r="B32" s="25" t="s">
         <v>821</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="B33" s="25" t="s">
         <v>823</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="B34" s="25" t="s">
         <v>825</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="306" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
+        <v>826</v>
+      </c>
+      <c r="B35" s="25" t="s">
         <v>827</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
+        <v>828</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>829</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>830</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
+        <v>830</v>
+      </c>
+      <c r="B37" s="25" t="s">
         <v>831</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>832</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>834</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>836</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
+        <v>837</v>
+      </c>
+      <c r="B41" s="25" t="s">
         <v>838</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
+        <v>839</v>
+      </c>
+      <c r="B42" s="25" t="s">
         <v>840</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
+        <v>841</v>
+      </c>
+      <c r="B43" s="25" t="s">
         <v>842</v>
-      </c>
-      <c r="B43" s="25" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
+        <v>843</v>
+      </c>
+      <c r="B44" s="25" t="s">
         <v>844</v>
-      </c>
-      <c r="B44" s="25" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
+        <v>845</v>
+      </c>
+      <c r="B45" s="25" t="s">
         <v>846</v>
-      </c>
-      <c r="B45" s="25" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="B46" s="25" t="s">
         <v>848</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>849</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="B47" s="25" t="s">
         <v>850</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>851</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="221" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
+        <v>852</v>
+      </c>
+      <c r="B49" s="25" t="s">
         <v>853</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
+        <v>854</v>
+      </c>
+      <c r="B50" s="25" t="s">
         <v>855</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
+        <v>856</v>
+      </c>
+      <c r="B51" s="25" t="s">
         <v>857</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
+        <v>858</v>
+      </c>
+      <c r="B52" s="25" t="s">
         <v>859</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="102" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
+        <v>860</v>
+      </c>
+      <c r="B53" s="25" t="s">
         <v>861</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
+        <v>862</v>
+      </c>
+      <c r="B54" s="25" t="s">
         <v>863</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
+        <v>864</v>
+      </c>
+      <c r="B55" s="25" t="s">
         <v>865</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="221" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="B56" s="25" t="s">
         <v>867</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
+        <v>868</v>
+      </c>
+      <c r="B57" s="25" t="s">
         <v>869</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
+        <v>870</v>
+      </c>
+      <c r="B58" s="25" t="s">
         <v>871</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
+        <v>872</v>
+      </c>
+      <c r="B59" s="25" t="s">
         <v>873</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
+        <v>874</v>
+      </c>
+      <c r="B60" s="25" t="s">
         <v>875</v>
-      </c>
-      <c r="B60" s="25" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
+        <v>876</v>
+      </c>
+      <c r="B61" s="25" t="s">
         <v>877</v>
-      </c>
-      <c r="B61" s="25" t="s">
-        <v>878</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
+        <v>879</v>
+      </c>
+      <c r="B63" s="25" t="s">
         <v>880</v>
-      </c>
-      <c r="B63" s="25" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
+        <v>881</v>
+      </c>
+      <c r="B64" s="25" t="s">
         <v>882</v>
-      </c>
-      <c r="B64" s="25" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="289" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
+        <v>883</v>
+      </c>
+      <c r="B65" s="25" t="s">
         <v>884</v>
-      </c>
-      <c r="B65" s="25" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
+        <v>885</v>
+      </c>
+      <c r="B66" s="25" t="s">
         <v>886</v>
-      </c>
-      <c r="B66" s="25" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
+        <v>887</v>
+      </c>
+      <c r="B67" s="25" t="s">
         <v>888</v>
-      </c>
-      <c r="B67" s="25" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="B68" s="25" t="s">
         <v>890</v>
-      </c>
-      <c r="B68" s="25" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="B69" s="25" t="s">
         <v>892</v>
-      </c>
-      <c r="B69" s="25" t="s">
-        <v>893</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
+        <v>893</v>
+      </c>
+      <c r="B70" s="25" t="s">
         <v>894</v>
-      </c>
-      <c r="B70" s="25" t="s">
-        <v>895</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
+        <v>895</v>
+      </c>
+      <c r="B71" s="25" t="s">
         <v>896</v>
-      </c>
-      <c r="B71" s="25" t="s">
-        <v>897</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
+        <v>897</v>
+      </c>
+      <c r="B72" s="25" t="s">
         <v>898</v>
-      </c>
-      <c r="B72" s="25" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="238" x14ac:dyDescent="0.2">
       <c r="A73" s="7" t="s">
+        <v>899</v>
+      </c>
+      <c r="B73" s="25" t="s">
         <v>900</v>
-      </c>
-      <c r="B73" s="25" t="s">
-        <v>901</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="153" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
+        <v>901</v>
+      </c>
+      <c r="B74" s="25" t="s">
         <v>902</v>
-      </c>
-      <c r="B74" s="25" t="s">
-        <v>903</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="7" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B75" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B76" s="25" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="7" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="B78" s="25" t="s">
         <v>907</v>
-      </c>
-      <c r="B78" s="25" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="7" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="B80" s="25" t="s">
         <v>910</v>
-      </c>
-      <c r="B80" s="25" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="7" t="s">
+        <v>911</v>
+      </c>
+      <c r="B81" s="25" t="s">
         <v>912</v>
-      </c>
-      <c r="B81" s="25" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
+        <v>913</v>
+      </c>
+      <c r="B82" s="25" t="s">
         <v>914</v>
-      </c>
-      <c r="B82" s="25" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="153" x14ac:dyDescent="0.2">
       <c r="A83" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="B83" s="25" t="s">
         <v>916</v>
-      </c>
-      <c r="B83" s="25" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
+        <v>918</v>
+      </c>
+      <c r="B85" s="25" t="s">
         <v>919</v>
-      </c>
-      <c r="B85" s="25" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B86" s="25"/>
     </row>
     <row r="87" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
+        <v>921</v>
+      </c>
+      <c r="B87" s="25" t="s">
         <v>922</v>
-      </c>
-      <c r="B87" s="25" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B88" s="25"/>
     </row>
     <row r="89" spans="1:2" ht="51" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="B89" s="25" t="s">
         <v>925</v>
-      </c>
-      <c r="B89" s="25" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
+        <v>927</v>
+      </c>
+      <c r="B91" s="25" t="s">
         <v>928</v>
-      </c>
-      <c r="B91" s="25" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="92" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
+        <v>929</v>
+      </c>
+      <c r="B92" s="25" t="s">
         <v>930</v>
-      </c>
-      <c r="B92" s="25" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="93" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="B93" s="25" t="s">
         <v>932</v>
-      </c>
-      <c r="B93" s="25" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
+        <v>934</v>
+      </c>
+      <c r="B95" s="25" t="s">
         <v>935</v>
-      </c>
-      <c r="B95" s="25" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="96" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
+        <v>936</v>
+      </c>
+      <c r="B96" s="25" t="s">
         <v>937</v>
-      </c>
-      <c r="B96" s="25" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
+        <v>939</v>
+      </c>
+      <c r="B98" s="25" t="s">
         <v>940</v>
-      </c>
-      <c r="B98" s="25" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="99" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A99" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="B99" s="25" t="s">
         <v>942</v>
-      </c>
-      <c r="B99" s="25" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="100" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="B100" s="25" t="s">
         <v>944</v>
-      </c>
-      <c r="B100" s="25" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="101" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="B101" s="25" t="s">
         <v>946</v>
-      </c>
-      <c r="B101" s="25" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="102" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
+        <v>947</v>
+      </c>
+      <c r="B102" s="25" t="s">
         <v>948</v>
-      </c>
-      <c r="B102" s="25" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="103" spans="1:2" ht="119" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
+        <v>949</v>
+      </c>
+      <c r="B103" s="25" t="s">
         <v>950</v>
-      </c>
-      <c r="B103" s="25" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="104" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
+        <v>951</v>
+      </c>
+      <c r="B104" s="40" t="s">
         <v>952</v>
-      </c>
-      <c r="B104" s="40" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="105" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
+        <v>953</v>
+      </c>
+      <c r="B105" s="25" t="s">
         <v>954</v>
-      </c>
-      <c r="B105" s="25" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="106" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
+        <v>955</v>
+      </c>
+      <c r="B106" s="25" t="s">
         <v>956</v>
-      </c>
-      <c r="B106" s="25" t="s">
-        <v>957</v>
       </c>
     </row>
     <row r="107" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A107" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="B107" s="25" t="s">
         <v>958</v>
-      </c>
-      <c r="B107" s="25" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="108" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="B108" s="25" t="s">
         <v>960</v>
-      </c>
-      <c r="B108" s="25" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="109" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="B109" s="25" t="s">
         <v>962</v>
-      </c>
-      <c r="B109" s="25" t="s">
-        <v>963</v>
       </c>
     </row>
     <row r="110" spans="1:2" ht="68" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="B110" s="25" t="s">
         <v>964</v>
-      </c>
-      <c r="B110" s="25" t="s">
-        <v>965</v>
       </c>
     </row>
     <row r="111" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A111" s="7" t="s">
+        <v>965</v>
+      </c>
+      <c r="B111" s="25" t="s">
         <v>966</v>
-      </c>
-      <c r="B111" s="25" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="112" spans="1:2" ht="136" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
+        <v>967</v>
+      </c>
+      <c r="B112" s="25" t="s">
         <v>968</v>
-      </c>
-      <c r="B112" s="25" t="s">
-        <v>969</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="221" x14ac:dyDescent="0.2">
       <c r="A113" s="7" t="s">
+        <v>969</v>
+      </c>
+      <c r="B113" s="25" t="s">
         <v>970</v>
-      </c>
-      <c r="B113" s="25" t="s">
-        <v>971</v>
       </c>
     </row>
   </sheetData>
@@ -11258,24 +11258,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
+        <v>971</v>
+      </c>
+      <c r="C1" s="24" t="s">
         <v>972</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="D1" s="14" t="s">
         <v>973</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="24" t="s">
         <v>974</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="F1" s="14" t="s">
         <v>975</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B2" s="41">
         <v>0</v>
@@ -11284,7 +11284,7 @@
         <v>629</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>629</v>
@@ -11295,7 +11295,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B3" s="41">
         <v>1</v>
@@ -11304,7 +11304,7 @@
         <v>42</v>
       </c>
       <c r="D3" s="42" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>42</v>
@@ -11315,7 +11315,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B4" s="41">
         <v>2</v>
@@ -11324,7 +11324,7 @@
         <v>42</v>
       </c>
       <c r="D4" s="42" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>42</v>
@@ -11335,7 +11335,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B5" s="41">
         <v>3</v>
@@ -11344,7 +11344,7 @@
         <v>42</v>
       </c>
       <c r="D5" s="42" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>42</v>
@@ -11355,16 +11355,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="B6" s="43" t="s">
         <v>985</v>
       </c>
-      <c r="B6" s="43" t="s">
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="42" t="s">
         <v>986</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="42" t="s">
-        <v>987</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>42</v>
@@ -11375,16 +11375,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B7" s="43" t="s">
         <v>988</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="C7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="42" t="s">
         <v>989</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D7" s="42" t="s">
-        <v>990</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>42</v>
@@ -11395,16 +11395,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="B8" s="43" t="s">
         <v>991</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="42" t="s">
         <v>992</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D8" s="42" t="s">
-        <v>993</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>42</v>
@@ -11415,7 +11415,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="B9" s="41">
         <v>4</v>
@@ -11424,7 +11424,7 @@
         <v>42</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>42</v>
@@ -11435,7 +11435,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B10" s="41">
         <v>5</v>
@@ -11444,7 +11444,7 @@
         <v>42</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>42</v>
@@ -11455,16 +11455,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="B11" s="43" t="s">
         <v>998</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="C11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="42" t="s">
         <v>999</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="42" t="s">
-        <v>1000</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>42</v>
@@ -11475,16 +11475,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B12" s="43" t="s">
         <v>1001</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="42" t="s">
         <v>1002</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" s="42" t="s">
-        <v>1003</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>42</v>
@@ -11495,16 +11495,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B13" s="43" t="s">
         <v>1004</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="C13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="42" t="s">
         <v>1005</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="42" t="s">
-        <v>1006</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>42</v>
@@ -11515,16 +11515,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B14" s="43" t="s">
         <v>1007</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="42" t="s">
         <v>1008</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="42" t="s">
-        <v>1009</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>42</v>
@@ -11535,16 +11535,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B15" s="43" t="s">
         <v>1010</v>
       </c>
-      <c r="B15" s="43" t="s">
+      <c r="C15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="42" t="s">
         <v>1011</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="42" t="s">
-        <v>1012</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>42</v>
@@ -11555,7 +11555,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B16" s="41">
         <v>6</v>
@@ -11564,7 +11564,7 @@
         <v>42</v>
       </c>
       <c r="D16" s="42" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>42</v>
@@ -11575,16 +11575,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B17" s="43" t="s">
         <v>1015</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="C17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="42" t="s">
         <v>1016</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="42" t="s">
-        <v>1017</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>42</v>
@@ -11595,16 +11595,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B18" s="43" t="s">
         <v>1018</v>
       </c>
-      <c r="B18" s="43" t="s">
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="42" t="s">
         <v>1019</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>1020</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>42</v>
@@ -11615,16 +11615,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="B19" s="43" t="s">
         <v>1021</v>
       </c>
-      <c r="B19" s="43" t="s">
+      <c r="C19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="42" t="s">
         <v>1022</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="42" t="s">
-        <v>1023</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>42</v>
@@ -11635,16 +11635,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>1023</v>
+      </c>
+      <c r="B20" s="43" t="s">
         <v>1024</v>
       </c>
-      <c r="B20" s="43" t="s">
+      <c r="C20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="42" t="s">
         <v>1025</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>1026</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>42</v>
@@ -11655,16 +11655,16 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="B21" s="43" t="s">
         <v>1027</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="C21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="42" t="s">
         <v>1028</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="42" t="s">
-        <v>1029</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>42</v>
@@ -11675,10 +11675,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B22" s="43" t="s">
         <v>1030</v>
-      </c>
-      <c r="B22" s="43" t="s">
-        <v>1031</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>42</v>
@@ -11695,16 +11695,16 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B23" s="43" t="s">
         <v>1032</v>
       </c>
-      <c r="B23" s="43" t="s">
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="42" t="s">
         <v>1033</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="42" t="s">
-        <v>1034</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>42</v>
@@ -11715,16 +11715,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B24" s="43" t="s">
         <v>1035</v>
       </c>
-      <c r="B24" s="43" t="s">
+      <c r="C24" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D24" s="42" t="s">
         <v>1036</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="42" t="s">
-        <v>1037</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>42</v>
@@ -11735,7 +11735,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B25" s="41">
         <v>7</v>
@@ -11744,7 +11744,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="42" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>42</v>
@@ -11755,16 +11755,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="B26" s="43" t="s">
         <v>1040</v>
       </c>
-      <c r="B26" s="43" t="s">
+      <c r="C26" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="42" t="s">
         <v>1041</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>1042</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>42</v>
@@ -11775,207 +11775,207 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B27" s="43" t="s">
         <v>1043</v>
       </c>
-      <c r="B27" s="43" t="s">
+      <c r="C27" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D27" s="42" t="s">
         <v>1044</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="42" t="s">
-        <v>1045</v>
-      </c>
       <c r="E27" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="B28" s="43" t="s">
         <v>1046</v>
       </c>
-      <c r="B28" s="43" t="s">
+      <c r="C28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="42" t="s">
         <v>1047</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="42" t="s">
-        <v>1048</v>
-      </c>
       <c r="E28" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="B29" s="43" t="s">
         <v>1049</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="C29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="42" t="s">
         <v>1050</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="42" t="s">
-        <v>1051</v>
-      </c>
       <c r="E29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="B30" s="43" t="s">
         <v>1052</v>
       </c>
-      <c r="B30" s="43" t="s">
+      <c r="C30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" s="42" t="s">
         <v>1053</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="42" t="s">
-        <v>1054</v>
-      </c>
       <c r="E30" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B31" s="43" t="s">
         <v>1055</v>
       </c>
-      <c r="B31" s="43" t="s">
+      <c r="C31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D31" s="42" t="s">
         <v>1056</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>1057</v>
-      </c>
       <c r="E31" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
+        <v>1057</v>
+      </c>
+      <c r="B32" s="43" t="s">
         <v>1058</v>
       </c>
-      <c r="B32" s="43" t="s">
+      <c r="C32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="42" t="s">
         <v>1059</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="42" t="s">
-        <v>1060</v>
-      </c>
       <c r="E32" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="B33" s="43" t="s">
         <v>1061</v>
       </c>
-      <c r="B33" s="43" t="s">
+      <c r="C33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" s="42" t="s">
         <v>1062</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D33" s="42" t="s">
-        <v>1063</v>
-      </c>
       <c r="E33" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="B34" s="43" t="s">
         <v>1064</v>
       </c>
-      <c r="B34" s="43" t="s">
+      <c r="C34" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="42" t="s">
         <v>1065</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D34" s="42" t="s">
-        <v>1066</v>
-      </c>
       <c r="E34" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B35" s="43" t="s">
         <v>1067</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="C35" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="42" t="s">
         <v>1068</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="42" t="s">
-        <v>1069</v>
-      </c>
       <c r="E35" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B36" s="43" t="s">
         <v>1070</v>
       </c>
-      <c r="B36" s="43" t="s">
+      <c r="C36" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="42" t="s">
         <v>1071</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="42" t="s">
-        <v>1072</v>
-      </c>
       <c r="E36" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B37" s="41">
         <v>8</v>
@@ -11984,118 +11984,118 @@
         <v>42</v>
       </c>
       <c r="D37" s="42" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B38" s="43" t="s">
         <v>1075</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="C38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="42" t="s">
         <v>1076</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="42" t="s">
-        <v>1077</v>
-      </c>
       <c r="E38" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="B39" s="43" t="s">
         <v>1078</v>
       </c>
-      <c r="B39" s="43" t="s">
+      <c r="C39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="42" t="s">
         <v>1079</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D39" s="42" t="s">
-        <v>1080</v>
-      </c>
       <c r="E39" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B40" s="43" t="s">
         <v>1081</v>
       </c>
-      <c r="B40" s="43" t="s">
+      <c r="C40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D40" s="42" t="s">
         <v>1082</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D40" s="42" t="s">
-        <v>1083</v>
-      </c>
       <c r="E40" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B41" s="43" t="s">
         <v>1084</v>
       </c>
-      <c r="B41" s="43" t="s">
+      <c r="C41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" s="42" t="s">
         <v>1085</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D41" s="42" t="s">
-        <v>1086</v>
-      </c>
       <c r="E41" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
+        <v>1086</v>
+      </c>
+      <c r="B42" s="43" t="s">
         <v>1087</v>
       </c>
-      <c r="B42" s="43" t="s">
+      <c r="C42" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="42" t="s">
         <v>1088</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" s="42" t="s">
-        <v>1089</v>
-      </c>
       <c r="E42" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B43" s="41">
         <v>9</v>
@@ -12104,421 +12104,421 @@
         <v>42</v>
       </c>
       <c r="D43" s="42" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B44" s="43" t="s">
         <v>1092</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="C44" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" s="42" t="s">
         <v>1093</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="42" t="s">
-        <v>1094</v>
-      </c>
       <c r="E44" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="B45" s="43" t="s">
         <v>1095</v>
       </c>
-      <c r="B45" s="43" t="s">
+      <c r="C45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D45" s="42" t="s">
         <v>1096</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D45" s="42" t="s">
-        <v>1097</v>
-      </c>
       <c r="E45" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="B46" s="43" t="s">
         <v>1098</v>
       </c>
-      <c r="B46" s="43" t="s">
+      <c r="C46" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D46" s="42" t="s">
         <v>1099</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D46" s="42" t="s">
-        <v>1100</v>
-      </c>
       <c r="E46" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B47" s="43" t="s">
         <v>1101</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="C47" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="42" t="s">
         <v>1102</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D47" s="42" t="s">
-        <v>1103</v>
-      </c>
       <c r="E47" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B48" s="43" t="s">
         <v>1104</v>
       </c>
-      <c r="B48" s="43" t="s">
+      <c r="C48" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="42" t="s">
         <v>1105</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D48" s="42" t="s">
-        <v>1106</v>
-      </c>
       <c r="E48" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B49" s="43" t="s">
         <v>1107</v>
       </c>
-      <c r="B49" s="43" t="s">
+      <c r="C49" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D49" s="42" t="s">
         <v>1108</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>1109</v>
-      </c>
       <c r="E49" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B50" s="43" t="s">
         <v>1110</v>
       </c>
-      <c r="B50" s="43" t="s">
+      <c r="C50" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="42" t="s">
         <v>1111</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D50" s="42" t="s">
-        <v>1112</v>
-      </c>
       <c r="E50" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B51" s="43" t="s">
         <v>1113</v>
       </c>
-      <c r="B51" s="43" t="s">
+      <c r="C51" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D51" s="42" t="s">
         <v>1114</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D51" s="42" t="s">
-        <v>1115</v>
-      </c>
       <c r="E51" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B52" s="43" t="s">
         <v>1116</v>
       </c>
-      <c r="B52" s="43" t="s">
+      <c r="C52" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="42" t="s">
         <v>1117</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D52" s="42" t="s">
-        <v>1118</v>
-      </c>
       <c r="E52" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B53" s="43" t="s">
         <v>1119</v>
       </c>
-      <c r="B53" s="43" t="s">
+      <c r="C53" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D53" s="42" t="s">
         <v>1120</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D53" s="42" t="s">
-        <v>1121</v>
-      </c>
       <c r="E53" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B54" s="43" t="s">
         <v>1122</v>
       </c>
-      <c r="B54" s="43" t="s">
+      <c r="C54" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="44" t="s">
         <v>1123</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D54" s="44" t="s">
-        <v>1124</v>
-      </c>
       <c r="E54" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B55" s="43" t="s">
         <v>1125</v>
       </c>
-      <c r="B55" s="43" t="s">
+      <c r="C55" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D55" s="42" t="s">
         <v>1126</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D55" s="42" t="s">
-        <v>1127</v>
-      </c>
       <c r="E55" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B56" s="43" t="s">
         <v>1128</v>
       </c>
-      <c r="B56" s="43" t="s">
+      <c r="C56" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D56" s="42" t="s">
         <v>1129</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="42" t="s">
-        <v>1130</v>
-      </c>
       <c r="E56" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B57" s="43" t="s">
         <v>1131</v>
       </c>
-      <c r="B57" s="43" t="s">
+      <c r="C57" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="42" t="s">
         <v>1132</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D57" s="42" t="s">
-        <v>1133</v>
-      </c>
       <c r="E57" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B58" s="43" t="s">
         <v>1134</v>
       </c>
-      <c r="B58" s="43" t="s">
+      <c r="C58" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D58" s="42" t="s">
         <v>1135</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D58" s="42" t="s">
-        <v>1136</v>
-      </c>
       <c r="E58" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B59" s="43" t="s">
         <v>1137</v>
       </c>
-      <c r="B59" s="43" t="s">
+      <c r="C59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="42" t="s">
         <v>1138</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D59" s="42" t="s">
-        <v>1139</v>
-      </c>
       <c r="E59" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="B60" s="43" t="s">
         <v>1140</v>
       </c>
-      <c r="B60" s="43" t="s">
+      <c r="C60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D60" s="42" t="s">
         <v>1141</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D60" s="42" t="s">
-        <v>1142</v>
-      </c>
       <c r="E60" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B61" s="43" t="s">
         <v>1143</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="C61" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" s="42" t="s">
         <v>1144</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D61" s="42" t="s">
-        <v>1145</v>
-      </c>
       <c r="E61" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B62" s="43" t="s">
         <v>1146</v>
       </c>
-      <c r="B62" s="43" t="s">
+      <c r="C62" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D62" s="42" t="s">
         <v>1147</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D62" s="42" t="s">
-        <v>1148</v>
-      </c>
       <c r="E62" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="B63" s="43" t="s">
         <v>1149</v>
       </c>
-      <c r="B63" s="43" t="s">
+      <c r="C63" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D63" s="42" t="s">
         <v>1150</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D63" s="42" t="s">
-        <v>1151</v>
-      </c>
       <c r="E63" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B64" s="43" t="s">
         <v>1152</v>
-      </c>
-      <c r="B64" s="43" t="s">
-        <v>1153</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>42</v>
@@ -12530,252 +12530,252 @@
         <v>42</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B65" s="43" t="s">
         <v>1154</v>
       </c>
-      <c r="B65" s="43" t="s">
+      <c r="C65" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D65" s="42" t="s">
         <v>1155</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D65" s="42" t="s">
-        <v>1156</v>
-      </c>
       <c r="E65" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B66" s="43" t="s">
         <v>1157</v>
       </c>
-      <c r="B66" s="43" t="s">
+      <c r="C66" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="42" t="s">
         <v>1158</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D66" s="42" t="s">
-        <v>1159</v>
-      </c>
       <c r="E66" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B67" s="43" t="s">
         <v>1160</v>
       </c>
-      <c r="B67" s="43" t="s">
+      <c r="C67" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="42" t="s">
         <v>1161</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D67" s="42" t="s">
-        <v>1162</v>
-      </c>
       <c r="E67" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B68" s="43" t="s">
         <v>1163</v>
       </c>
-      <c r="B68" s="43" t="s">
+      <c r="C68" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D68" s="42" t="s">
         <v>1164</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D68" s="42" t="s">
-        <v>1165</v>
-      </c>
       <c r="E68" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="B69" s="43" t="s">
         <v>1166</v>
       </c>
-      <c r="B69" s="43" t="s">
+      <c r="C69" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D69" s="42" t="s">
         <v>1167</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="42" t="s">
-        <v>1168</v>
-      </c>
       <c r="E69" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B70" s="43" t="s">
         <v>1169</v>
       </c>
-      <c r="B70" s="43" t="s">
+      <c r="C70" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D70" s="42" t="s">
         <v>1170</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D70" s="42" t="s">
-        <v>1171</v>
-      </c>
       <c r="E70" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B71" s="43" t="s">
         <v>1172</v>
       </c>
-      <c r="B71" s="43" t="s">
+      <c r="C71" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D71" s="42" t="s">
         <v>1173</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D71" s="42" t="s">
-        <v>1174</v>
-      </c>
       <c r="E71" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B72" s="43" t="s">
         <v>1175</v>
       </c>
-      <c r="B72" s="43" t="s">
+      <c r="C72" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="42" t="s">
         <v>1176</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D72" s="42" t="s">
-        <v>1177</v>
-      </c>
       <c r="E72" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B73" s="43" t="s">
         <v>1178</v>
       </c>
-      <c r="B73" s="43" t="s">
+      <c r="C73" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D73" s="42" t="s">
         <v>1179</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D73" s="42" t="s">
-        <v>1180</v>
-      </c>
       <c r="E73" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B74" s="43" t="s">
         <v>1181</v>
       </c>
-      <c r="B74" s="43" t="s">
+      <c r="C74" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D74" s="42" t="s">
         <v>1182</v>
       </c>
-      <c r="C74" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D74" s="42" t="s">
-        <v>1183</v>
-      </c>
       <c r="E74" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B75" s="43" t="s">
         <v>1184</v>
       </c>
-      <c r="B75" s="43" t="s">
+      <c r="C75" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D75" s="42" t="s">
         <v>1185</v>
       </c>
-      <c r="C75" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D75" s="42" t="s">
-        <v>1186</v>
-      </c>
       <c r="E75" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B76" s="43" t="s">
         <v>1187</v>
       </c>
-      <c r="B76" s="43" t="s">
+      <c r="C76" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D76" s="42" t="s">
         <v>1188</v>
       </c>
-      <c r="C76" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D76" s="42" t="s">
-        <v>1189</v>
-      </c>
       <c r="E76" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="B77" s="41">
         <v>10</v>
@@ -12784,538 +12784,538 @@
         <v>42</v>
       </c>
       <c r="D77" s="42" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E77" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B78" s="43" t="s">
         <v>1192</v>
       </c>
-      <c r="B78" s="43" t="s">
+      <c r="C78" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D78" s="42" t="s">
         <v>1193</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D78" s="42" t="s">
-        <v>1194</v>
-      </c>
       <c r="E78" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B79" s="43" t="s">
         <v>1195</v>
       </c>
-      <c r="B79" s="43" t="s">
+      <c r="C79" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D79" s="42" t="s">
         <v>1196</v>
       </c>
-      <c r="C79" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D79" s="42" t="s">
-        <v>1197</v>
-      </c>
       <c r="E79" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B80" s="43" t="s">
         <v>1198</v>
       </c>
-      <c r="B80" s="43" t="s">
+      <c r="C80" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D80" s="42" t="s">
         <v>1199</v>
       </c>
-      <c r="C80" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D80" s="42" t="s">
-        <v>1200</v>
-      </c>
       <c r="E80" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
+        <v>1200</v>
+      </c>
+      <c r="B81" s="43" t="s">
         <v>1201</v>
       </c>
-      <c r="B81" s="43" t="s">
+      <c r="C81" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D81" s="42" t="s">
         <v>1202</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D81" s="42" t="s">
-        <v>1203</v>
-      </c>
       <c r="E81" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B82" s="43" t="s">
         <v>1204</v>
       </c>
-      <c r="B82" s="43" t="s">
-        <v>1205</v>
-      </c>
       <c r="C82" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D82" s="42" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B83" s="43" t="s">
         <v>1206</v>
       </c>
-      <c r="B83" s="43" t="s">
+      <c r="C83" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D83" s="42" t="s">
         <v>1207</v>
       </c>
-      <c r="C83" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D83" s="42" t="s">
-        <v>1208</v>
-      </c>
       <c r="E83" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="B84" s="43" t="s">
         <v>1209</v>
       </c>
-      <c r="B84" s="43" t="s">
+      <c r="C84" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D84" s="42" t="s">
         <v>1210</v>
       </c>
-      <c r="C84" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D84" s="42" t="s">
-        <v>1211</v>
-      </c>
       <c r="E84" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B85" s="43" t="s">
         <v>1212</v>
       </c>
-      <c r="B85" s="43" t="s">
+      <c r="C85" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D85" s="42" t="s">
         <v>1213</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D85" s="42" t="s">
-        <v>1214</v>
-      </c>
       <c r="E85" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="B86" s="43" t="s">
         <v>1215</v>
       </c>
-      <c r="B86" s="43" t="s">
+      <c r="C86" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D86" s="45" t="s">
         <v>1216</v>
       </c>
-      <c r="C86" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D86" s="45" t="s">
-        <v>1217</v>
-      </c>
       <c r="E86" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B87" s="43" t="s">
         <v>1218</v>
       </c>
-      <c r="B87" s="43" t="s">
+      <c r="C87" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="45" t="s">
         <v>1219</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D87" s="45" t="s">
-        <v>1220</v>
-      </c>
       <c r="E87" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B88" s="43" t="s">
         <v>1221</v>
       </c>
-      <c r="B88" s="43" t="s">
+      <c r="C88" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D88" s="42" t="s">
         <v>1222</v>
       </c>
-      <c r="C88" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D88" s="42" t="s">
-        <v>1223</v>
-      </c>
       <c r="E88" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="B89" s="43" t="s">
         <v>1224</v>
       </c>
-      <c r="B89" s="43" t="s">
+      <c r="C89" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D89" s="42" t="s">
         <v>1225</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D89" s="42" t="s">
-        <v>1226</v>
-      </c>
       <c r="E89" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B90" s="43" t="s">
         <v>1227</v>
       </c>
-      <c r="B90" s="43" t="s">
+      <c r="C90" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D90" s="42" t="s">
         <v>1228</v>
       </c>
-      <c r="C90" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D90" s="42" t="s">
-        <v>1229</v>
-      </c>
       <c r="E90" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B91" s="43" t="s">
         <v>1230</v>
       </c>
-      <c r="B91" s="43" t="s">
+      <c r="C91" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D91" s="42" t="s">
         <v>1231</v>
       </c>
-      <c r="C91" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D91" s="42" t="s">
-        <v>1232</v>
-      </c>
       <c r="E91" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B92" s="43" t="s">
         <v>1233</v>
       </c>
-      <c r="B92" s="43" t="s">
+      <c r="C92" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D92" s="42" t="s">
         <v>1234</v>
       </c>
-      <c r="C92" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D92" s="42" t="s">
-        <v>1235</v>
-      </c>
       <c r="E92" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="B93" s="43" t="s">
         <v>1236</v>
       </c>
-      <c r="B93" s="43" t="s">
+      <c r="C93" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D93" s="42" t="s">
         <v>1237</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D93" s="42" t="s">
-        <v>1238</v>
-      </c>
       <c r="E93" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B94" s="43" t="s">
         <v>1239</v>
       </c>
-      <c r="B94" s="43" t="s">
+      <c r="C94" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D94" s="42" t="s">
         <v>1240</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D94" s="42" t="s">
-        <v>1241</v>
-      </c>
       <c r="E94" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="B95" s="43" t="s">
         <v>1242</v>
       </c>
-      <c r="B95" s="43" t="s">
+      <c r="C95" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D95" s="42" t="s">
         <v>1243</v>
       </c>
-      <c r="C95" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D95" s="42" t="s">
-        <v>1244</v>
-      </c>
       <c r="E95" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B96" s="43" t="s">
         <v>1245</v>
       </c>
-      <c r="B96" s="43" t="s">
+      <c r="C96" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D96" s="42" t="s">
         <v>1246</v>
       </c>
-      <c r="C96" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D96" s="42" t="s">
-        <v>1247</v>
-      </c>
       <c r="E96" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B97" s="43" t="s">
         <v>1248</v>
       </c>
-      <c r="B97" s="43" t="s">
+      <c r="C97" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D97" s="42" t="s">
         <v>1249</v>
       </c>
-      <c r="C97" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D97" s="42" t="s">
-        <v>1250</v>
-      </c>
       <c r="E97" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B98" s="43" t="s">
         <v>1251</v>
       </c>
-      <c r="B98" s="43" t="s">
+      <c r="C98" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D98" s="42" t="s">
         <v>1252</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D98" s="42" t="s">
-        <v>1253</v>
-      </c>
       <c r="E98" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B99" s="43" t="s">
         <v>1254</v>
       </c>
-      <c r="B99" s="43" t="s">
+      <c r="C99" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D99" s="42" t="s">
         <v>1255</v>
       </c>
-      <c r="C99" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D99" s="42" t="s">
-        <v>1256</v>
-      </c>
       <c r="E99" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B100" s="43" t="s">
         <v>1257</v>
       </c>
-      <c r="B100" s="43" t="s">
+      <c r="C100" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D100" s="42" t="s">
         <v>1258</v>
       </c>
-      <c r="C100" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D100" s="42" t="s">
-        <v>1259</v>
-      </c>
       <c r="E100" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B101" s="43" t="s">
         <v>1260</v>
       </c>
-      <c r="B101" s="43" t="s">
+      <c r="C101" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D101" s="42" t="s">
         <v>1261</v>
       </c>
-      <c r="C101" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D101" s="42" t="s">
-        <v>1262</v>
-      </c>
       <c r="E101" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B102" s="43" t="s">
         <v>1263</v>
       </c>
-      <c r="B102" s="43" t="s">
+      <c r="C102" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D102" s="42" t="s">
         <v>1264</v>
       </c>
-      <c r="C102" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D102" s="42" t="s">
-        <v>1265</v>
-      </c>
       <c r="E102" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B103" s="43" t="s">
         <v>1266</v>
       </c>
-      <c r="B103" s="43" t="s">
+      <c r="C103" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D103" s="42" t="s">
         <v>1267</v>
       </c>
-      <c r="C103" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D103" s="42" t="s">
-        <v>1268</v>
-      </c>
       <c r="E103" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>1269</v>
+        <v>1268</v>
       </c>
       <c r="B104" s="41">
         <v>11</v>
@@ -13324,161 +13324,161 @@
         <v>42</v>
       </c>
       <c r="D104" s="42" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B105" s="43" t="s">
         <v>1271</v>
       </c>
-      <c r="B105" s="43" t="s">
+      <c r="C105" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D105" s="42" t="s">
         <v>1272</v>
       </c>
-      <c r="C105" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D105" s="42" t="s">
-        <v>1273</v>
-      </c>
       <c r="E105" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B106" s="43" t="s">
         <v>1274</v>
       </c>
-      <c r="B106" s="43" t="s">
+      <c r="C106" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D106" s="42" t="s">
         <v>1275</v>
       </c>
-      <c r="C106" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D106" s="42" t="s">
-        <v>1276</v>
-      </c>
       <c r="E106" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="B107" s="43" t="s">
         <v>1277</v>
       </c>
-      <c r="B107" s="43" t="s">
+      <c r="C107" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D107" s="42" t="s">
         <v>1278</v>
       </c>
-      <c r="C107" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D107" s="42" t="s">
-        <v>1279</v>
-      </c>
       <c r="E107" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B108" s="43" t="s">
         <v>1280</v>
       </c>
-      <c r="B108" s="43" t="s">
+      <c r="C108" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D108" s="42" t="s">
         <v>1281</v>
       </c>
-      <c r="C108" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D108" s="42" t="s">
-        <v>1282</v>
-      </c>
       <c r="E108" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B109" s="43" t="s">
         <v>1283</v>
       </c>
-      <c r="B109" s="43" t="s">
+      <c r="C109" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D109" s="42" t="s">
         <v>1284</v>
       </c>
-      <c r="C109" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D109" s="42" t="s">
-        <v>1285</v>
-      </c>
       <c r="E109" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="B110" s="43" t="s">
         <v>1286</v>
       </c>
-      <c r="B110" s="43" t="s">
-        <v>1287</v>
-      </c>
       <c r="C110" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D110" s="42" t="s">
-        <v>1235</v>
+        <v>1234</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="B111" s="43" t="s">
         <v>1288</v>
       </c>
-      <c r="B111" s="43" t="s">
+      <c r="C111" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D111" s="42" t="s">
         <v>1289</v>
       </c>
-      <c r="C111" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D111" s="42" t="s">
-        <v>1290</v>
-      </c>
       <c r="E111" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B112" s="43" t="s">
         <v>1291</v>
-      </c>
-      <c r="B112" s="43" t="s">
-        <v>1292</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>42</v>
@@ -13490,27 +13490,27 @@
         <v>42</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="113" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B113" s="43" t="s">
         <v>1293</v>
       </c>
-      <c r="B113" s="43" t="s">
+      <c r="C113" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D113" s="44" t="s">
         <v>1294</v>
       </c>
-      <c r="C113" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D113" s="44" t="s">
-        <v>1295</v>
-      </c>
       <c r="E113" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F113" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
   </sheetData>

</xml_diff>